<commit_message>
code ref on pos
</commit_message>
<xml_diff>
--- a/procurement_export_pos.xlsx
+++ b/procurement_export_pos.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\fas2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10790"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Republic of  the Philippines</t>
   </si>
@@ -29,15 +33,14 @@
     <t>BIDS AND AWARDS COMMITTEE</t>
   </si>
   <si>
-    <t>Annaliza Mendoza Banawa</t>
-  </si>
-  <si>
-    <t>ACCESS WATER INTEGRATORS AND EQUIPMENT PHILS. INC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Unit B9 2nd Floor Regalena Bldg. National Highway Brgy. Turbina
-Calamba City
+    <t>Ms. Maria Lanlet Cajipe Arzola</t>
+  </si>
+  <si>
+    <t>1-Air Master Enterprise, Inc.</t>
+  </si>
+  <si>
+    <t>#94 P. Paterno St. Brgy. Dela Paz, BiÃƒÂ±an City, Laguna.
+BiÃƒÂ±an
 Laguna</t>
   </si>
   <si>
@@ -50,33 +53,24 @@
     <t>RFQ NO.</t>
   </si>
   <si>
-    <t>2022-0003</t>
+    <t>2023-00005</t>
   </si>
   <si>
     <t>Approved Budget for the Contract (ABC)</t>
   </si>
   <si>
-    <t>PHP65,500.00</t>
+    <t>PHP3,000.00</t>
   </si>
   <si>
     <t>Purpose</t>
   </si>
   <si>
-    <t>LOREM IPSUM</t>
+    <t>d</t>
   </si>
   <si>
     <t>End User</t>
   </si>
   <si>
-    <t>ORD</t>
-  </si>
-  <si>
-    <t>For further inquiries, you may contact the BAC Secretariat Office at (049) 827-3143 or dilg4a.bac@gmail.com</t>
-  </si>
-  <si>
-    <t>Thank you.</t>
-  </si>
-  <si>
     <t>Prepared by:</t>
   </si>
   <si>
@@ -96,60 +90,47 @@
   </si>
   <si>
     <t>Received by:</t>
+  </si>
+  <si>
+    <t>For further inquiries, you may contact the BAC Secretariat Office at (02) 8-876-3454 loc. 7410 or dilg4a.bac@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,21 +138,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="7">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -186,32 +174,43 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -221,87 +220,84 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -317,7 +313,7 @@
     <xdr:ext cx="752475" cy="762000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -329,7 +325,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -626,81 +625,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="160" view="pageLayout" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A31" zoomScale="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="22"/>
-    <col min="2" max="2" width="8.109375" customWidth="true" style="2"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="13.6640625" customWidth="true" style="2"/>
-    <col min="9" max="9" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.90625" style="5"/>
+    <col min="2" max="2" width="8.08984375" style="2" customWidth="1"/>
+    <col min="3" max="7" width="8.90625" style="2"/>
+    <col min="8" max="8" width="13.6328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="E1" s="2"/>
-    </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="C7" s="7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C8" s="1"/>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="C11" s="17"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -714,7 +703,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -728,7 +717,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -742,7 +731,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -754,7 +743,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -766,7 +755,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -780,7 +769,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -792,7 +781,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -806,10 +795,10 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" customHeight="1" ht="2.4">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+    <row r="21" spans="1:10" ht="2.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -818,107 +807,105 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" customHeight="1" ht="16.2">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:10" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="19" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" customHeight="1" ht="28.2">
-      <c r="A23" s="20" t="s">
+    <row r="23" spans="1:10" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="10" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="16"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="10"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -930,35 +917,33 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+    <row r="30" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -969,7 +954,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -981,23 +966,23 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1009,39 +994,39 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="6" t="s">
-        <v>21</v>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1053,7 +1038,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1065,7 +1050,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1077,9 +1062,9 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1091,7 +1076,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1103,13 +1088,13 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1117,7 +1102,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1129,7 +1114,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1142,8 +1127,14 @@
       <c r="J45" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="16">
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="D24:I27"/>
+    <mergeCell ref="A24:C27"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:I28"/>
@@ -1153,24 +1144,10 @@
     <mergeCell ref="D22:I22"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="D24:I27"/>
-    <mergeCell ref="A24:C27"/>
+    <mergeCell ref="A30:I31"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>